<commit_message>
Bereich 'Abteilung' zur Datenbank und 'Nutzer'-Methode '_existenz_boolean_daten_feststellen' + entsprechende Tests  hinzugefügt. Datenimport und alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
+++ b/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBEC255-BC65-44E0-ACFC-D47618891FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3A1093-CAFD-4DA7-8DC7-60BA37F410E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -217,6 +218,42 @@
   </si>
   <si>
     <t>Werkstudent</t>
+  </si>
+  <si>
+    <t>Abteilungsabkürzung</t>
+  </si>
+  <si>
+    <t>Personalcontrolling</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Führungskraft</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>maennlich</t>
+  </si>
+  <si>
+    <t>divers</t>
+  </si>
+  <si>
+    <t>Angestellter</t>
+  </si>
+  <si>
+    <t>Arbeiter</t>
+  </si>
+  <si>
+    <t>Auszubildender</t>
+  </si>
+  <si>
+    <t>Praktikant</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -633,9 +670,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -863,154 +900,299 @@
       <c r="B25" s="8">
         <v>35</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="B29" s="2"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="D28" s="11"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
+      <c r="B30" s="7"/>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="D29" s="11"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="B31" s="7"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="D30" s="11"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+      <c r="B32" s="13"/>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="9"/>
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B34" s="5"/>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="5"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="15"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="2"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="7"/>
+      <c r="A42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="2"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="7"/>
+      <c r="A43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="2"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B44" s="7"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B45" s="7"/>
       <c r="D45" s="11"/>
     </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="D47" s="11"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{ADD7711E-89F9-4C61-8272-4BC0124032CE}">
+      <formula1>0</formula1>
+      <formula2>60</formula2>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1" xr:uid="{71AFB16E-529B-4436-B8EE-EE56A3A5D5CA}"/>
     <hyperlink ref="B14" r:id="rId2" xr:uid="{37BFBA39-2674-4F74-BA9A-74B241690977}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E880C197-BC95-4C5B-A656-6C63E902724E}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCDEDDF9-8147-443B-8508-A6C8D922FCA7}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7DA73FF-D468-4194-9329-301A08ACE2B5}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$E$2:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A420BD95-21E4-42A6-83BB-B7592398D91C}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B28</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41E031-B515-4B55-B38F-F0D31894393C}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bereich 'Jobtitel' in Datenbank inkl. entsprechende Stored Procedures erstellt. Datenimport und alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
+++ b/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3A1093-CAFD-4DA7-8DC7-60BA37F410E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C7BB39-FEAB-4812-9921-0182406C59F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>ja</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Anzahl Kinder</t>
   </si>
 </sst>
 </file>
@@ -670,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +889,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -909,7 +918,7 @@
       <c r="B26" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
@@ -918,7 +927,7 @@
       <c r="B27" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
@@ -927,27 +936,31 @@
       <c r="B28" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="D29" s="11"/>
+      <c r="A29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="D30" s="11"/>
+        <v>38</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="7"/>
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="2"/>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1061,6 +1074,13 @@
       </c>
       <c r="B47" s="7"/>
       <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="D48" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Bereich 'Gesellschaft' inkl. entsprechende Stored Procedures hinzugefuegt. Datenimport und alle Tests laufen.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
+++ b/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C7BB39-FEAB-4812-9921-0182406C59F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39263101-1C51-4E4D-B529-E91EB8640214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -220,9 +220,6 @@
     <t>Werkstudent</t>
   </si>
   <si>
-    <t>Abteilungsabkürzung</t>
-  </si>
-  <si>
     <t>Personalcontrolling</t>
   </si>
   <si>
@@ -263,6 +260,18 @@
   </si>
   <si>
     <t>Anzahl Kinder</t>
+  </si>
+  <si>
+    <t>Abkuerzung Abteilung</t>
+  </si>
+  <si>
+    <t>Abkuerzung Gesellschaft</t>
+  </si>
+  <si>
+    <t>Berliner Stadtreinigung</t>
+  </si>
+  <si>
+    <t>BSR</t>
   </si>
 </sst>
 </file>
@@ -679,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,7 +898,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -916,25 +925,25 @@
         <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -943,7 +952,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -952,135 +961,146 @@
         <v>38</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+      <c r="B31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="B33" s="13"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="5"/>
+      <c r="B34" s="9"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B35" s="5"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="5"/>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="5"/>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="15"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B40" s="2"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="2"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="7"/>
+      <c r="A44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="2"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B45" s="7"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="7"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B47" s="7"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B48" s="7"/>
       <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="D49" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1149,7 +1169,7 @@
         <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1157,32 +1177,32 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>63</v>
@@ -1193,7 +1213,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1201,7 +1221,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6">
         <v>5</v>

</xml_diff>

<commit_message>
SELECT-Befehl können unter Beachtung von RLS korrekt übergeben werden. Mandanten und Nutzer erstellen eigene Connection zur Datenbank. Alle Unit-Tests entsprechend angepasst und laufen erfolgreich.
</commit_message>
<xml_diff>
--- a/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
+++ b/src/main/Mitarbeiterdaten/Erika Musterfrau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Mitarbeiterdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39263101-1C51-4E4D-B529-E91EB8640214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AEEF13-3C81-4CE0-9F3B-CFFB0C786ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>Personalnummer</t>
   </si>
   <si>
-    <t>M100001</t>
-  </si>
-  <si>
     <t>01.01.2024</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t>BSR</t>
+  </si>
+  <si>
+    <t>M100002</t>
   </si>
 </sst>
 </file>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +713,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D2" s="10"/>
     </row>
@@ -722,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -738,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -756,7 +756,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -862,7 +862,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -871,7 +871,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="10"/>
     </row>
@@ -886,25 +886,25 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="14">
         <v>1</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="8">
         <v>35</v>
@@ -922,182 +922,182 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="13"/>
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="5"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="5"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="5"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" s="15"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="2"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="2"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="2"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="2"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="7"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="7"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="7"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="7"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" s="7"/>
       <c r="D49" s="11"/>
@@ -1160,52 +1160,52 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6">
         <v>5</v>

</xml_diff>